<commit_message>
add day mean columns
</commit_message>
<xml_diff>
--- a/static/template.xlsx
+++ b/static/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjgong/WorkSpace/Code/pm25image/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjgong/WorkSpace/Code/pm25image/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5961E603-7502-5D46-A436-75C2B631FD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FBE893-88A7-5A44-B340-4C78B025068F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="680" windowWidth="27860" windowHeight="15960" xr2:uid="{D26F2FB5-EE4F-A14D-8462-C17E57B646D3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <r>
       <rPr>
@@ -322,6 +322,14 @@
   </si>
   <si>
     <t>序号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当日累计</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -374,7 +382,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -397,13 +405,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -419,20 +521,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -761,322 +920,475 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F145D7-7548-2843-AE62-7C419AC80D75}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" customWidth="1"/>
-    <col min="3" max="5" width="18.83203125" customWidth="1"/>
+    <col min="1" max="8" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="16" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="7">
         <v>44516.5</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="38" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="32" customHeight="1">
+      <c r="A2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4">
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" customHeight="1">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" customHeight="1">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C4" s="4">
         <v>59</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D4" s="5">
+        <v>59</v>
+      </c>
+      <c r="E4" s="4">
         <v>102</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F4" s="5">
+        <v>59</v>
+      </c>
+      <c r="G4" s="5">
+        <v>59</v>
+      </c>
+      <c r="H4" s="4">
         <v>47</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4">
+    </row>
+    <row r="5" spans="1:8" ht="16" customHeight="1">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <v>78</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="5">
+        <v>78</v>
+      </c>
+      <c r="E5" s="4">
         <v>138</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F5" s="5">
+        <v>78</v>
+      </c>
+      <c r="G5" s="5">
+        <v>78</v>
+      </c>
+      <c r="H5" s="4">
         <v>49</v>
       </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4">
+    </row>
+    <row r="6" spans="1:8" ht="16" customHeight="1">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>83</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="5">
+        <v>83</v>
+      </c>
+      <c r="E6" s="4">
         <v>163</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F6" s="5">
+        <v>83</v>
+      </c>
+      <c r="G6" s="5">
+        <v>83</v>
+      </c>
+      <c r="H6" s="4">
         <v>64</v>
       </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4">
+    </row>
+    <row r="7" spans="1:8" ht="16" customHeight="1">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>63</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="5">
+        <v>63</v>
+      </c>
+      <c r="E7" s="4">
         <v>136</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F7" s="5">
+        <v>63</v>
+      </c>
+      <c r="G7" s="5">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4">
         <v>56</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4">
+    </row>
+    <row r="8" spans="1:8" ht="16" customHeight="1">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>68</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="5">
+        <v>68</v>
+      </c>
+      <c r="E8" s="4">
         <v>124</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F8" s="5">
+        <v>68</v>
+      </c>
+      <c r="G8" s="5">
+        <v>68</v>
+      </c>
+      <c r="H8" s="4">
         <v>48</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="4">
+    </row>
+    <row r="9" spans="1:8" ht="16" customHeight="1">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4">
         <v>139</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4">
         <v>68</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="4">
+    </row>
+    <row r="10" spans="1:8" ht="16" customHeight="1">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>53</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="5">
+        <v>53</v>
+      </c>
+      <c r="E10" s="4">
         <v>102</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F10" s="5">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5">
+        <v>53</v>
+      </c>
+      <c r="H10" s="4">
         <v>56</v>
       </c>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="4">
+    </row>
+    <row r="11" spans="1:8" ht="16" customHeight="1">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C11" s="4">
         <v>75</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D11" s="5">
+        <v>75</v>
+      </c>
+      <c r="E11" s="4">
         <v>156</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F11" s="5">
+        <v>75</v>
+      </c>
+      <c r="G11" s="5">
+        <v>75</v>
+      </c>
+      <c r="H11" s="4">
         <v>45</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="4">
+    </row>
+    <row r="12" spans="1:8" ht="16" customHeight="1">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C12" s="4">
         <v>78</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D12" s="5">
+        <v>78</v>
+      </c>
+      <c r="E12" s="4">
         <v>117</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F12" s="5">
+        <v>78</v>
+      </c>
+      <c r="G12" s="5">
+        <v>78</v>
+      </c>
+      <c r="H12" s="4">
         <v>57</v>
       </c>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="4">
+    </row>
+    <row r="13" spans="1:8" ht="16" customHeight="1">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <v>70</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D13" s="5">
+        <v>70</v>
+      </c>
+      <c r="E13" s="4">
         <v>134</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F13" s="5">
+        <v>70</v>
+      </c>
+      <c r="G13" s="5">
+        <v>70</v>
+      </c>
+      <c r="H13" s="4">
         <v>88</v>
       </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="4">
+    </row>
+    <row r="14" spans="1:8" ht="16" customHeight="1">
+      <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>77</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D14" s="5">
+        <v>77</v>
+      </c>
+      <c r="E14" s="4">
         <v>141</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F14" s="5">
+        <v>77</v>
+      </c>
+      <c r="G14" s="5">
+        <v>77</v>
+      </c>
+      <c r="H14" s="4">
         <v>71</v>
       </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4">
+    </row>
+    <row r="15" spans="1:8" ht="16" customHeight="1">
+      <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C15" s="4">
         <v>87</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D15" s="5">
+        <v>87</v>
+      </c>
+      <c r="E15" s="4">
         <v>129</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F15" s="5">
+        <v>87</v>
+      </c>
+      <c r="G15" s="5">
+        <v>87</v>
+      </c>
+      <c r="H15" s="4">
         <v>58</v>
       </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="4">
+    </row>
+    <row r="16" spans="1:8" ht="16" customHeight="1">
+      <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C16" s="4">
         <v>59</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D16" s="5">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4">
         <v>104</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F16" s="5">
+        <v>59</v>
+      </c>
+      <c r="G16" s="5">
+        <v>59</v>
+      </c>
+      <c r="H16" s="4">
         <v>66</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="17" spans="1:8" ht="16" customHeight="1">
+      <c r="A17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="3">
-        <f>ROUND(AVERAGE(C3:C15),0)</f>
+      <c r="B17" s="6"/>
+      <c r="C17" s="3">
+        <f>ROUND(AVERAGE(C4:C16),0)</f>
         <v>71</v>
       </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:E16" si="0">ROUND(AVERAGE(D3:D15),0)</f>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:H17" si="0">ROUND(AVERAGE(D4:D16),0)</f>
+        <v>71</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F17" s="3">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="H17" s="3">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A16:B16"/>
+  <mergeCells count="7">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="C3:C15">
+  <conditionalFormatting sqref="C4:C16">
+    <cfRule type="top10" dxfId="5" priority="6" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E16">
+    <cfRule type="top10" dxfId="4" priority="5" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H4:H16">
+    <cfRule type="top10" dxfId="3" priority="4" rank="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D16">
     <cfRule type="top10" dxfId="2" priority="3" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D15">
+  <conditionalFormatting sqref="F4:F16">
     <cfRule type="top10" dxfId="1" priority="2" rank="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E15">
+  <conditionalFormatting sqref="G4:G16">
     <cfRule type="top10" dxfId="0" priority="1" rank="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>